<commit_message>
minor fix to data dictionary
</commit_message>
<xml_diff>
--- a/data_dictionary/data_dic_2019.xlsx
+++ b/data_dictionary/data_dic_2019.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Proj_acess_oport\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r1701707\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="Port" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="196">
   <si>
     <t>sigla_muni</t>
   </si>
@@ -607,10 +607,16 @@
     <t>Travel time from to the closest healthcare facility with low complextiy services</t>
   </si>
   <si>
-    <t>v1, 20190116</t>
-  </si>
-  <si>
     <t>Organization of the columns with accessibility estimates</t>
+  </si>
+  <si>
+    <t>Valor = Inf quando tempo de viagem for maior do que 2h (transporte público) ou 1,5h (a pé ou de bicicleta)</t>
+  </si>
+  <si>
+    <t>Value = Inf when travel time is longer than 2h (public transport) or 1,5h (walking or bicycle)</t>
+  </si>
+  <si>
+    <t>v1, 20200116</t>
   </si>
 </sst>
 </file>
@@ -687,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -728,12 +734,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1038,15 +1038,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21.75">
       <c r="A2" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="26"/>
+        <v>195</v>
+      </c>
+      <c r="B2" s="24"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" thickBot="1">
@@ -1430,14 +1430,16 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="2:5" ht="30" customHeight="1" thickBot="1">
-      <c r="B41" s="19" t="s">
+    <row r="41" spans="2:5" ht="29.25" thickBot="1">
+      <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D41" s="20"/>
+      <c r="D41" s="15" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="17"/>
@@ -1445,20 +1447,20 @@
       <c r="D42" s="17"/>
     </row>
     <row r="43" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="20"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="10" t="s">
@@ -1486,7 +1488,7 @@
         <v>66</v>
       </c>
       <c r="D47" s="11"/>
-      <c r="E47" s="23"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="10" t="s">
@@ -1561,9 +1563,9 @@
       <c r="D55" s="8"/>
     </row>
     <row r="56" spans="2:4">
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="2:4" ht="15.75" thickBot="1">
       <c r="B57" s="4" t="s">
@@ -1573,18 +1575,18 @@
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="20" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="59" spans="2:4">
-      <c r="B59" s="24">
+      <c r="B59" s="22">
         <v>15</v>
       </c>
       <c r="C59" s="11" t="s">
@@ -1595,7 +1597,7 @@
       </c>
     </row>
     <row r="60" spans="2:4">
-      <c r="B60" s="24">
+      <c r="B60" s="22">
         <v>30</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -1606,7 +1608,7 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="24">
+      <c r="B61" s="22">
         <v>45</v>
       </c>
       <c r="C61" s="11" t="s">
@@ -1617,7 +1619,7 @@
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62" s="24">
+      <c r="B62" s="22">
         <v>60</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -1628,7 +1630,7 @@
       </c>
     </row>
     <row r="63" spans="2:4">
-      <c r="B63" s="24">
+      <c r="B63" s="22">
         <v>90</v>
       </c>
       <c r="C63" s="11" t="s">
@@ -1639,7 +1641,7 @@
       </c>
     </row>
     <row r="64" spans="2:4" ht="15" thickBot="1">
-      <c r="B64" s="25">
+      <c r="B64" s="23">
         <v>120</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -1691,15 +1693,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21.75">
       <c r="A2" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="26"/>
+        <v>195</v>
+      </c>
+      <c r="B2" s="24"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" thickBot="1">
@@ -2051,7 +2053,7 @@
     </row>
     <row r="34" spans="2:5" ht="15">
       <c r="B34" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -2095,13 +2097,15 @@
       <c r="D40" s="6"/>
     </row>
     <row r="41" spans="2:5" ht="30" customHeight="1" thickBot="1">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="20"/>
+      <c r="D41" s="15" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="17"/>
@@ -2109,20 +2113,20 @@
       <c r="D42" s="17"/>
     </row>
     <row r="43" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="20" t="s">
         <v>154</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="20"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="10" t="s">
@@ -2150,7 +2154,7 @@
         <v>158</v>
       </c>
       <c r="D47" s="11"/>
-      <c r="E47" s="23"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="10" t="s">
@@ -2225,9 +2229,9 @@
       <c r="D55" s="8"/>
     </row>
     <row r="56" spans="2:4">
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="2:4" ht="15.75" thickBot="1">
       <c r="B57" s="4" t="s">
@@ -2237,18 +2241,18 @@
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>168</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="20" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="59" spans="2:4">
-      <c r="B59" s="24">
+      <c r="B59" s="22">
         <v>15</v>
       </c>
       <c r="C59" s="11" t="s">
@@ -2259,7 +2263,7 @@
       </c>
     </row>
     <row r="60" spans="2:4">
-      <c r="B60" s="24">
+      <c r="B60" s="22">
         <v>30</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -2270,7 +2274,7 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="24">
+      <c r="B61" s="22">
         <v>45</v>
       </c>
       <c r="C61" s="11" t="s">
@@ -2281,7 +2285,7 @@
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62" s="24">
+      <c r="B62" s="22">
         <v>60</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -2292,7 +2296,7 @@
       </c>
     </row>
     <row r="63" spans="2:4">
-      <c r="B63" s="24">
+      <c r="B63" s="22">
         <v>90</v>
       </c>
       <c r="C63" s="11" t="s">
@@ -2303,7 +2307,7 @@
       </c>
     </row>
     <row r="64" spans="2:4" ht="15" thickBot="1">
-      <c r="B64" s="25">
+      <c r="B64" s="23">
         <v>120</v>
       </c>
       <c r="C64" s="8" t="s">

</xml_diff>